<commit_message>
Uploading new TEP, Artelys, and Agora files
</commit_message>
<xml_diff>
--- a/InputData/trans/BRASC/BAU Rng Anxiety Shadow Costs.xlsx
+++ b/InputData/trans/BRASC/BAU Rng Anxiety Shadow Costs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,7 +22,7 @@
     <definedName name="Range_EV">Calculations!$B$9</definedName>
     <definedName name="range_ICE">Calculations!$B$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +34,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -65,127 +67,127 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
+    <t>BRAaCTSC BAU Range Anxiety Shadow Cost</t>
+  </si>
+  <si>
     <t>Source:</t>
   </si>
   <si>
+    <t>Median US Income</t>
+  </si>
+  <si>
+    <t>United States Census Bureau</t>
+  </si>
+  <si>
+    <t>Income and Poverty in the United States: 2019</t>
+  </si>
+  <si>
+    <t>https://www.census.gov/library/publications/2020/demo/p60-270.html</t>
+  </si>
+  <si>
+    <t>First bullet of "Highlights"</t>
+  </si>
+  <si>
+    <t>Range and Fueling Availability 'Costs'</t>
+  </si>
+  <si>
+    <t>US Department of Energy</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy13osti/55639.pdf</t>
+  </si>
+  <si>
+    <t>Gasoline vehicle range</t>
+  </si>
+  <si>
+    <t>All-Electric Vehicle Ranges Can Exceed Those of Some Gasoline Vehicles</t>
+  </si>
+  <si>
+    <t>https://www.energy.gov/eere/vehicles/fact-939-august-22-2016-all-electric-vehicle-ranges-can-exceed-those-some-gasoline</t>
+  </si>
+  <si>
+    <t>First Figure</t>
+  </si>
+  <si>
+    <t>EV range</t>
+  </si>
+  <si>
+    <t>Inside Evs</t>
+  </si>
+  <si>
+    <t>The Median Range of Fully Electric Vehicles Exceeded 250 Miles in 2020</t>
+  </si>
+  <si>
+    <t>https://insideevs.com/news/464449/median-range-evs-2020-exceeded-250-miles/</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>This variable represents the perceived cost of range anxiety - the fear (or inconvenience around) that</t>
+  </si>
+  <si>
+    <t>the vehicle has insufficient range to reach its destination.</t>
+  </si>
+  <si>
+    <t>In the US, we use a DOE study to calculate a Range Compensating Value and a Fuel Availability Value.</t>
+  </si>
+  <si>
+    <t>The Range Compensating Value uses parameters from the DOE study, the median household income,</t>
+  </si>
+  <si>
+    <t>and the median ranges of ICE and EV vehicles. For EV vehicles, the current median range has already surpassed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250 miles and is forecated to continue improving. Therefore, we start with today's median range, and assume </t>
+  </si>
+  <si>
+    <t>the range will reach 300 miles by 2050.</t>
+  </si>
+  <si>
+    <t>Currency Conversion</t>
+  </si>
+  <si>
+    <t>2019 to 2012 USD</t>
+  </si>
+  <si>
+    <t>Range Compensating Value</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>median range ice (hundred miles)</t>
+  </si>
+  <si>
+    <t>range ev (hundred miles)</t>
+  </si>
+  <si>
+    <t>income (thousand USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2020 median range taken from historical data. 2030 and 2050 are estimated, with the 2050 </t>
+  </si>
+  <si>
+    <t>range roughly corresponding to today's maximum range</t>
+  </si>
+  <si>
+    <t>cv (thousand USD)</t>
+  </si>
+  <si>
+    <t>Cost ($/vehicle)</t>
+  </si>
+  <si>
     <t>Shadow cost</t>
-  </si>
-  <si>
-    <t>This variable represents the perceived cost of range anxiety - the fear (or inconvenience around) that</t>
-  </si>
-  <si>
-    <t>the vehicle has insufficient range to reach its destination.</t>
-  </si>
-  <si>
-    <t>Cost ($/vehicle)</t>
-  </si>
-  <si>
-    <t>income (thousand USD)</t>
-  </si>
-  <si>
-    <t>range ev (hundred miles)</t>
-  </si>
-  <si>
-    <t>b4</t>
-  </si>
-  <si>
-    <t>b3</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>Range Compensating Value</t>
-  </si>
-  <si>
-    <t>cv (thousand USD)</t>
-  </si>
-  <si>
-    <t>https://www.census.gov/library/publications/2020/demo/p60-270.html</t>
-  </si>
-  <si>
-    <t>Median US Income</t>
-  </si>
-  <si>
-    <t>United States Census Bureau</t>
-  </si>
-  <si>
-    <t>Income and Poverty in the United States: 2019</t>
-  </si>
-  <si>
-    <t>First bullet of "Highlights"</t>
-  </si>
-  <si>
-    <t>2019 to 2012 USD</t>
-  </si>
-  <si>
-    <t>Range and Fueling Availability 'Costs'</t>
-  </si>
-  <si>
-    <t>US Department of Energy</t>
-  </si>
-  <si>
-    <t>https://www.nrel.gov/docs/fy13osti/55639.pdf</t>
-  </si>
-  <si>
-    <t>Gasoline vehicle range</t>
-  </si>
-  <si>
-    <t>All-Electric Vehicle Ranges Can Exceed Those of Some Gasoline Vehicles</t>
-  </si>
-  <si>
-    <t>https://www.energy.gov/eere/vehicles/fact-939-august-22-2016-all-electric-vehicle-ranges-can-exceed-those-some-gasoline</t>
-  </si>
-  <si>
-    <t>First Figure</t>
-  </si>
-  <si>
-    <t>median range ice (hundred miles)</t>
-  </si>
-  <si>
-    <t>Inside Evs</t>
-  </si>
-  <si>
-    <t>The Median Range of Fully Electric Vehicles Exceeded 250 Miles in 2020</t>
-  </si>
-  <si>
-    <t>https://insideevs.com/news/464449/median-range-evs-2020-exceeded-250-miles/</t>
-  </si>
-  <si>
-    <t>EV range</t>
-  </si>
-  <si>
-    <t>In the US, we use a DOE study to calculate a Range Compensating Value and a Fuel Availability Value.</t>
-  </si>
-  <si>
-    <t>The Range Compensating Value uses parameters from the DOE study, the median household income,</t>
-  </si>
-  <si>
-    <t>and the median ranges of ICE and EV vehicles. For EV vehicles, the current median range has already surpassed</t>
-  </si>
-  <si>
-    <t>Currency Conversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250 miles and is forecated to continue improving. Therefore, we start with today's median range, and assume </t>
-  </si>
-  <si>
-    <t>the range will reach 300 miles by 2050.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*2020 median range taken from historical data. 2030 and 2050 are estimated, with the 2050 </t>
-  </si>
-  <si>
-    <t>range roughly corresponding to today's maximum range</t>
-  </si>
-  <si>
-    <t>BRAaCTSC BAU Range Anxiety Shadow Cost</t>
   </si>
 </sst>
 </file>
@@ -195,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,9 +282,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal 3 2" xfId="2" xr:uid="{3F0B3957-5839-491A-BB84-14323CF38870}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,177 +566,177 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="B5" s="7">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="B12" s="7">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="B15" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="B17" s="7">
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="B18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="B19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="B22" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="B23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="B24" s="7">
         <v>2021</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="B25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="B26" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B38">
         <v>0.89805481563188172</v>
@@ -756,48 +758,48 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>-0.36099999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1.268</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>-0.11600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7">
         <v>2020</v>
       </c>
@@ -808,9 +810,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>4.12</v>
@@ -823,9 +825,9 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>2.59</v>
@@ -837,9 +839,9 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>68.703000000000003</v>
@@ -853,19 +855,19 @@
         <v>68.703000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
       </c>
       <c r="B14" s="5">
         <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)*About!$B$38</f>
@@ -897,14 +899,14 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B1" s="4">
         <v>2020</v>
@@ -1000,9 +1002,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" cm="1">
         <f t="array" ref="B2">TREND(Calculations!$B$14:$C$14,Calculations!$B$7:$C$7,B1)*1000*About!$B$38</f>
@@ -1133,4 +1135,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64654C39-0A0F-44C7-83CA-43ADD3524528}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07EF07C9-B363-4F59-8470-EEFB850024D4}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74A0EE28-4F47-4984-A986-DD23553A2D66}"/>
 </file>
</xml_diff>